<commit_message>
docs(excel): update excel files
</commit_message>
<xml_diff>
--- a/excel/abertura-chamado.xlsx
+++ b/excel/abertura-chamado.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="74">
   <si>
     <t>Origem</t>
   </si>
@@ -230,6 +230,9 @@
   </si>
   <si>
     <t>E-mail com anexo de link suspeito enviado para todo setor</t>
+  </si>
+  <si>
+    <t>2025-03-19</t>
   </si>
 </sst>
 </file>
@@ -239,12 +242,17 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <color theme="1"/>
@@ -270,18 +278,16 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -555,807 +561,807 @@
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="4">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3">
         <v>45662.0</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3">
         <v>45667.0</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="4">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3">
         <v>45691.0</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="4">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="3">
         <v>45692.0</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="4">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3">
         <v>45695.0</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
         <v>45697.0</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="4">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3">
         <v>45700.0</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="4">
+      <c r="A10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3">
         <v>45702.0</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="4">
+      <c r="A11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="3">
         <v>45703.0</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="4">
+      <c r="A12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="3">
         <v>45706.0</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="4">
+      <c r="A13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="3">
         <v>45708.0</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="4">
+      <c r="A14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="3">
         <v>45710.0</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="4">
+      <c r="A15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="3">
         <v>45713.0</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="4">
+      <c r="A16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="3">
         <v>45714.0</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="4">
+      <c r="A17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="3">
         <v>45716.0</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="18" ht="14.25" customHeight="1">
-      <c r="A18" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="4">
+      <c r="A18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="3">
         <v>45660.0</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G18" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
-      <c r="A19" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="4">
+      <c r="A19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="3">
         <v>45664.0</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="G19" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="4">
+      <c r="A20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="3">
         <v>45669.0</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G20" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="4">
+      <c r="A21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="3">
         <v>45672.0</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G21" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="4">
+      <c r="A22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="3">
         <v>45689.0</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="G22" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="4">
+      <c r="A23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="3">
         <v>45691.0</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="G23" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="4">
+      <c r="A24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="3">
         <v>45693.0</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="G24" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
-      <c r="A25" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="4">
+      <c r="A25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="3">
         <v>45694.0</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="G25" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
-      <c r="A26" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="4">
+      <c r="A26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="3">
         <v>45696.0</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="G26" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="27" ht="14.25" customHeight="1">
-      <c r="A27" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="4">
+      <c r="A27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="3">
         <v>45699.0</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F27" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="G27" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="28" ht="14.25" customHeight="1">
-      <c r="A28" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" s="4">
+      <c r="A28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="3">
         <v>45701.0</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E28" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="G28" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
-      <c r="A29" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" s="4">
+      <c r="A29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="3">
         <v>45704.0</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E29" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G29" s="3" t="s">
+      <c r="G29" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="30" ht="14.25" customHeight="1">
-      <c r="A30" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30" s="4">
+      <c r="A30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="3">
         <v>45707.0</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E30" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F30" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G30" s="3" t="s">
+      <c r="G30" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="31" ht="14.25" customHeight="1">
-      <c r="A31" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B31" s="4">
+      <c r="A31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="3">
         <v>45709.0</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G31" s="3" t="s">
+      <c r="G31" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
-      <c r="A32" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B32" s="4">
+      <c r="A32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="3">
         <v>45711.0</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E32" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F32" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="G32" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="33" ht="14.25" customHeight="1">
-      <c r="A33" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B33" s="4">
+      <c r="A33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="3">
         <v>45713.0</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F33" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G33" s="3" t="s">
+      <c r="G33" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="34" ht="14.25" customHeight="1">
-      <c r="A34" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B34" s="4">
+      <c r="A34" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="3">
         <v>45715.0</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E34" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F34" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G34" s="3" t="s">
+      <c r="G34" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1">
-      <c r="A35" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B35" s="4">
+      <c r="A35" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="3">
         <v>45718.0</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E35" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F35" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G35" s="3" t="s">
+      <c r="G35" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="36" ht="14.25" customHeight="1">
-      <c r="A36" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B36" s="4">
+      <c r="A36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="3">
         <v>45726.0</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E36" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="F36" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G36" s="3" t="s">
+      <c r="G36" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="37" ht="14.25" customHeight="1">
-      <c r="A37" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B37" s="4">
+      <c r="A37" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="3">
         <v>45736.0</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D37" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E37" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F37" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G37" s="3" t="s">
+      <c r="G37" s="2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1382,7 +1388,26 @@
         <v>31</v>
       </c>
     </row>
-    <row r="39" ht="14.25" customHeight="1"/>
+    <row r="39" ht="14.25" customHeight="1">
+      <c r="A39" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="40" ht="14.25" customHeight="1"/>
     <row r="41" ht="14.25" customHeight="1"/>
     <row r="42" ht="14.25" customHeight="1"/>
@@ -2345,6 +2370,7 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
     <row r="1001" ht="15.75" customHeight="1"/>
+    <row r="1002" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>